<commit_message>
business issue understanding, modeling
</commit_message>
<xml_diff>
--- a/DA_Business/project/p2_mailing/项目二：预测邮寄产品目录带来的收入增长/p1-mailinglist.xlsx
+++ b/DA_Business/project/p2_mailing/项目二：预测邮寄产品目录带来的收入增长/p1-mailinglist.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jun\udacity\DA_Business\project\p2_mailing\项目二：预测邮寄产品目录带来的收入增长\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFA3828-15F6-4AA7-9FA3-CD749128D9EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19174" windowHeight="7654" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p1-mailinglist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -1635,26 +1636,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -1662,7 +1663,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1670,7 +1671,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1678,35 +1679,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1714,7 +1715,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1722,14 +1723,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1737,14 +1738,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1752,7 +1753,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1760,15 +1761,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2118,48 +2126,48 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2436,14 +2444,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2481,7 +2491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2519,7 +2529,7 @@
         <v>0.30503580699999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2557,7 +2567,7 @@
         <v>0.472724537</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2595,7 +2605,7 @@
         <v>0.57888185000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2633,7 +2643,7 @@
         <v>0.30513781099999998</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2671,7 +2681,7 @@
         <v>0.38770585499999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2709,7 +2719,7 @@
         <v>0.267278293</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2747,7 +2757,7 @@
         <v>0.22173949400000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -2785,7 +2795,7 @@
         <v>0.19344714900000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2823,7 +2833,7 @@
         <v>0.25065761399999997</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2861,7 +2871,7 @@
         <v>0.26452315199999998</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2899,7 +2909,7 @@
         <v>0.190541402</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2937,7 +2947,7 @@
         <v>0.19154490499999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2975,7 +2985,7 @@
         <v>0.212284098</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3013,7 +3023,7 @@
         <v>0.27796209500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -3051,7 +3061,7 @@
         <v>0.26970955200000002</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -3089,7 +3099,7 @@
         <v>0.238435971</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -3127,7 +3137,7 @@
         <v>0.23297942399999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -3165,7 +3175,7 @@
         <v>0.21210828600000001</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -3203,7 +3213,7 @@
         <v>0.22160676600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -3241,7 +3251,7 @@
         <v>0.19171627499999999</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -3279,7 +3289,7 @@
         <v>0.326687748</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -3317,7 +3327,7 @@
         <v>0.23341563700000001</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -3355,7 +3365,7 @@
         <v>0.27304769400000001</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3393,7 +3403,7 @@
         <v>0.19725817300000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -3431,7 +3441,7 @@
         <v>0.62724496600000001</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -3469,7 +3479,7 @@
         <v>0.24007403299999999</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -3507,7 +3517,7 @@
         <v>0.25712037599999998</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -3545,7 +3555,7 @@
         <v>0.61307269399999997</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3583,7 +3593,7 @@
         <v>0.38621956099999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -3621,7 +3631,7 @@
         <v>0.38321151599999997</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -3659,7 +3669,7 @@
         <v>0.29298455800000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3697,7 +3707,7 @@
         <v>0.24377779299999999</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -3735,7 +3745,7 @@
         <v>0.40985869899999999</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -3773,7 +3783,7 @@
         <v>0.22907971799999999</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -3811,7 +3821,7 @@
         <v>0.35448979200000003</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -3849,7 +3859,7 @@
         <v>0.20120116699999999</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3887,7 +3897,7 @@
         <v>0.213904022</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -3925,7 +3935,7 @@
         <v>0.22415280500000001</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>104</v>
       </c>
@@ -3963,7 +3973,7 @@
         <v>0.19136229799999999</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -4001,7 +4011,7 @@
         <v>0.49015270799999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -4039,7 +4049,7 @@
         <v>0.39429266099999999</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>111</v>
       </c>
@@ -4077,7 +4087,7 @@
         <v>0.23105563900000001</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>114</v>
       </c>
@@ -4115,7 +4125,7 @@
         <v>0.481368976</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -4153,7 +4163,7 @@
         <v>0.18732610099999999</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>118</v>
       </c>
@@ -4191,7 +4201,7 @@
         <v>0.207404056</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -4229,7 +4239,7 @@
         <v>0.28427938699999999</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -4267,7 +4277,7 @@
         <v>0.202412487</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>125</v>
       </c>
@@ -4305,7 +4315,7 @@
         <v>0.74854627200000001</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -4343,7 +4353,7 @@
         <v>0.21154409499999999</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -4381,7 +4391,7 @@
         <v>0.190822935</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>131</v>
       </c>
@@ -4419,7 +4429,7 @@
         <v>0.28486938000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>133</v>
       </c>
@@ -4457,7 +4467,7 @@
         <v>0.36600523699999998</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>135</v>
       </c>
@@ -4495,7 +4505,7 @@
         <v>0.25531713499999997</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>137</v>
       </c>
@@ -4533,7 +4543,7 @@
         <v>0.50114359600000002</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>139</v>
       </c>
@@ -4571,7 +4581,7 @@
         <v>0.19502314300000001</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>141</v>
       </c>
@@ -4609,7 +4619,7 @@
         <v>0.194825795</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>144</v>
       </c>
@@ -4647,7 +4657,7 @@
         <v>0.99882496200000004</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>147</v>
       </c>
@@ -4685,7 +4695,7 @@
         <v>0.268190172</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>149</v>
       </c>
@@ -4723,7 +4733,7 @@
         <v>0.21355267999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>151</v>
       </c>
@@ -4761,7 +4771,7 @@
         <v>0.18643868099999999</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>153</v>
       </c>
@@ -4799,7 +4809,7 @@
         <v>0.204701043</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>155</v>
       </c>
@@ -4837,7 +4847,7 @@
         <v>0.19957677400000001</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>157</v>
       </c>
@@ -4875,7 +4885,7 @@
         <v>0.23578850800000001</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>160</v>
       </c>
@@ -4913,7 +4923,7 @@
         <v>0.206906695</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>162</v>
       </c>
@@ -4951,7 +4961,7 @@
         <v>0.20274335399999999</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>164</v>
       </c>
@@ -4989,7 +4999,7 @@
         <v>0.54112264600000004</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>166</v>
       </c>
@@ -5027,7 +5037,7 @@
         <v>0.25644796399999997</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>168</v>
       </c>
@@ -5065,7 +5075,7 @@
         <v>0.24255331899999999</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>170</v>
       </c>
@@ -5103,7 +5113,7 @@
         <v>0.246686406</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>172</v>
       </c>
@@ -5141,7 +5151,7 @@
         <v>0.1931495</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>174</v>
       </c>
@@ -5179,7 +5189,7 @@
         <v>0.200860496</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>176</v>
       </c>
@@ -5217,7 +5227,7 @@
         <v>0.31807552300000003</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>178</v>
       </c>
@@ -5255,7 +5265,7 @@
         <v>0.21379023799999999</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>180</v>
       </c>
@@ -5293,7 +5303,7 @@
         <v>0.434214031</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>182</v>
       </c>
@@ -5331,7 +5341,7 @@
         <v>0.56531730099999999</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -5369,7 +5379,7 @@
         <v>0.66242807199999998</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>186</v>
       </c>
@@ -5407,7 +5417,7 @@
         <v>0.19257263599999999</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>188</v>
       </c>
@@ -5445,7 +5455,7 @@
         <v>0.22685629299999999</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -5483,7 +5493,7 @@
         <v>0.20422359900000001</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>192</v>
       </c>
@@ -5521,7 +5531,7 @@
         <v>0.28931545800000003</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>194</v>
       </c>
@@ -5559,7 +5569,7 @@
         <v>0.26960356299999999</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>196</v>
       </c>
@@ -5597,7 +5607,7 @@
         <v>0.20965584400000001</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>198</v>
       </c>
@@ -5635,7 +5645,7 @@
         <v>0.60683109499999999</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>200</v>
       </c>
@@ -5673,7 +5683,7 @@
         <v>0.190932877</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>203</v>
       </c>
@@ -5711,7 +5721,7 @@
         <v>0.19657658</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>205</v>
       </c>
@@ -5749,7 +5759,7 @@
         <v>0.25236414000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>207</v>
       </c>
@@ -5787,7 +5797,7 @@
         <v>0.467544876</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>209</v>
       </c>
@@ -5825,7 +5835,7 @@
         <v>0.25396285200000002</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>211</v>
       </c>
@@ -5863,7 +5873,7 @@
         <v>0.28849132199999999</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>213</v>
       </c>
@@ -5901,7 +5911,7 @@
         <v>0.62312773099999996</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>215</v>
       </c>
@@ -5939,7 +5949,7 @@
         <v>0.40099553900000001</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -5977,7 +5987,7 @@
         <v>0.34728293399999999</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>219</v>
       </c>
@@ -6015,7 +6025,7 @@
         <v>0.34281482400000002</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>221</v>
       </c>
@@ -6053,7 +6063,7 @@
         <v>0.38533516400000001</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>223</v>
       </c>
@@ -6091,7 +6101,7 @@
         <v>0.90327840999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>225</v>
       </c>
@@ -6129,7 +6139,7 @@
         <v>0.20291081799999999</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>227</v>
       </c>
@@ -6167,7 +6177,7 @@
         <v>0.997198264</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>229</v>
       </c>
@@ -6205,7 +6215,7 @@
         <v>0.22978557399999999</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>231</v>
       </c>
@@ -6243,7 +6253,7 @@
         <v>0.41528256699999999</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>233</v>
       </c>
@@ -6281,7 +6291,7 @@
         <v>0.86891464500000004</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>235</v>
       </c>
@@ -6319,7 +6329,7 @@
         <v>0.22552014300000001</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>237</v>
       </c>
@@ -6357,7 +6367,7 @@
         <v>0.41548464299999999</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>239</v>
       </c>
@@ -6395,7 +6405,7 @@
         <v>0.198583021</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>241</v>
       </c>
@@ -6433,7 +6443,7 @@
         <v>0.696914637</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>243</v>
       </c>
@@ -6471,7 +6481,7 @@
         <v>0.194225433</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>245</v>
       </c>
@@ -6509,7 +6519,7 @@
         <v>0.38174172200000001</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>247</v>
       </c>
@@ -6547,7 +6557,7 @@
         <v>0.347213357</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>249</v>
       </c>
@@ -6585,7 +6595,7 @@
         <v>0.73594038100000003</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>251</v>
       </c>
@@ -6623,7 +6633,7 @@
         <v>0.20697764299999999</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>253</v>
       </c>
@@ -6661,7 +6671,7 @@
         <v>0.19342088399999999</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>255</v>
       </c>
@@ -6699,7 +6709,7 @@
         <v>0.190638001</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>257</v>
       </c>
@@ -6737,7 +6747,7 @@
         <v>0.36029085500000002</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>259</v>
       </c>
@@ -6775,7 +6785,7 @@
         <v>0.387358706</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>261</v>
       </c>
@@ -6813,7 +6823,7 @@
         <v>0.25736213000000002</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>263</v>
       </c>
@@ -6851,7 +6861,7 @@
         <v>0.728853007</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>265</v>
       </c>
@@ -6889,7 +6899,7 @@
         <v>0.295262829</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>267</v>
       </c>
@@ -6927,7 +6937,7 @@
         <v>0.407311372</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>269</v>
       </c>
@@ -6965,7 +6975,7 @@
         <v>0.19669056800000001</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>271</v>
       </c>
@@ -7003,7 +7013,7 @@
         <v>0.335099172</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>273</v>
       </c>
@@ -7041,7 +7051,7 @@
         <v>0.20886049400000001</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>275</v>
       </c>
@@ -7079,7 +7089,7 @@
         <v>0.20524916600000001</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>277</v>
       </c>
@@ -7117,7 +7127,7 @@
         <v>0.235958794</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>279</v>
       </c>
@@ -7155,7 +7165,7 @@
         <v>0.30889710399999998</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>281</v>
       </c>
@@ -7193,7 +7203,7 @@
         <v>0.192939324</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>283</v>
       </c>
@@ -7231,7 +7241,7 @@
         <v>0.20695392200000001</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>285</v>
       </c>
@@ -7269,7 +7279,7 @@
         <v>0.330272968</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>287</v>
       </c>
@@ -7307,7 +7317,7 @@
         <v>0.237013536</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>289</v>
       </c>
@@ -7345,7 +7355,7 @@
         <v>0.23443860899999999</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>291</v>
       </c>
@@ -7383,7 +7393,7 @@
         <v>0.251869285</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>293</v>
       </c>
@@ -7421,7 +7431,7 @@
         <v>0.30242839199999999</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>295</v>
       </c>
@@ -7459,7 +7469,7 @@
         <v>0.375563594</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>297</v>
       </c>
@@ -7497,7 +7507,7 @@
         <v>0.43239717700000002</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>299</v>
       </c>
@@ -7535,7 +7545,7 @@
         <v>0.25093504700000002</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>301</v>
       </c>
@@ -7573,7 +7583,7 @@
         <v>0.34201468200000001</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>303</v>
       </c>
@@ -7611,7 +7621,7 @@
         <v>0.53399279600000005</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>305</v>
       </c>
@@ -7649,7 +7659,7 @@
         <v>0.57185430800000003</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>307</v>
       </c>
@@ -7687,7 +7697,7 @@
         <v>0.52588586599999998</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>309</v>
       </c>
@@ -7725,7 +7735,7 @@
         <v>0.27945864100000001</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>311</v>
       </c>
@@ -7763,7 +7773,7 @@
         <v>0.33053641700000003</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>313</v>
       </c>
@@ -7801,7 +7811,7 @@
         <v>0.21394580499999999</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>315</v>
       </c>
@@ -7839,7 +7849,7 @@
         <v>0.74127199600000004</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>317</v>
       </c>
@@ -7877,7 +7887,7 @@
         <v>0.31208787999999998</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>319</v>
       </c>
@@ -7915,7 +7925,7 @@
         <v>0.23846350499999999</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>321</v>
       </c>
@@ -7953,7 +7963,7 @@
         <v>0.65268244499999994</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>323</v>
       </c>
@@ -7991,7 +8001,7 @@
         <v>0.25220889499999999</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>325</v>
       </c>
@@ -8029,7 +8039,7 @@
         <v>0.756017995</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>327</v>
       </c>
@@ -8067,7 +8077,7 @@
         <v>0.18899550800000001</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>329</v>
       </c>
@@ -8105,7 +8115,7 @@
         <v>0.1921786</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>331</v>
       </c>
@@ -8143,7 +8153,7 @@
         <v>0.28263343699999999</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>333</v>
       </c>
@@ -8181,7 +8191,7 @@
         <v>0.47244747599999998</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>335</v>
       </c>
@@ -8219,7 +8229,7 @@
         <v>0.18771602600000001</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>337</v>
       </c>
@@ -8257,7 +8267,7 @@
         <v>0.55884010100000003</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>339</v>
       </c>
@@ -8295,7 +8305,7 @@
         <v>0.98223442000000005</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>341</v>
       </c>
@@ -8333,7 +8343,7 @@
         <v>0.229408525</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>343</v>
       </c>
@@ -8371,7 +8381,7 @@
         <v>0.220976802</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>345</v>
       </c>
@@ -8409,7 +8419,7 @@
         <v>0.225151025</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>347</v>
       </c>
@@ -8447,7 +8457,7 @@
         <v>0.220348242</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>349</v>
       </c>
@@ -8485,7 +8495,7 @@
         <v>0.19937788000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>351</v>
       </c>
@@ -8523,7 +8533,7 @@
         <v>0.47103065399999999</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>353</v>
       </c>
@@ -8561,7 +8571,7 @@
         <v>0.37826958700000002</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>355</v>
       </c>
@@ -8599,7 +8609,7 @@
         <v>0.90311748999999997</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>357</v>
       </c>
@@ -8637,7 +8647,7 @@
         <v>0.477434953</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>359</v>
       </c>
@@ -8675,7 +8685,7 @@
         <v>0.240232948</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>361</v>
       </c>
@@ -8713,7 +8723,7 @@
         <v>0.20727762399999999</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>363</v>
       </c>
@@ -8751,7 +8761,7 @@
         <v>0.18738121999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>365</v>
       </c>
@@ -8789,7 +8799,7 @@
         <v>0.28540892899999998</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>367</v>
       </c>
@@ -8827,7 +8837,7 @@
         <v>0.212397898</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>369</v>
       </c>
@@ -8865,7 +8875,7 @@
         <v>0.69072920299999996</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>371</v>
       </c>
@@ -8903,7 +8913,7 @@
         <v>0.226231668</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>373</v>
       </c>
@@ -8941,7 +8951,7 @@
         <v>0.31573054699999997</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>375</v>
       </c>
@@ -8979,7 +8989,7 @@
         <v>0.62019947600000003</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>377</v>
       </c>
@@ -9017,7 +9027,7 @@
         <v>0.40871876899999998</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>379</v>
       </c>
@@ -9055,7 +9065,7 @@
         <v>0.20889311799999999</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>381</v>
       </c>
@@ -9093,7 +9103,7 @@
         <v>0.23043298200000001</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>383</v>
       </c>
@@ -9131,7 +9141,7 @@
         <v>0.38457783499999998</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>385</v>
       </c>
@@ -9169,7 +9179,7 @@
         <v>0.42744749799999998</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>387</v>
       </c>
@@ -9207,7 +9217,7 @@
         <v>0.27713596600000001</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>389</v>
       </c>
@@ -9245,7 +9255,7 @@
         <v>0.92694539799999998</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>391</v>
       </c>
@@ -9283,7 +9293,7 @@
         <v>0.211074821</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>393</v>
       </c>
@@ -9321,7 +9331,7 @@
         <v>0.36646952500000002</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>395</v>
       </c>
@@ -9359,7 +9369,7 @@
         <v>0.196525851</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>397</v>
       </c>
@@ -9397,7 +9407,7 @@
         <v>0.185729488</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>399</v>
       </c>
@@ -9435,7 +9445,7 @@
         <v>0.37762712399999998</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>402</v>
       </c>
@@ -9473,7 +9483,7 @@
         <v>0.99999792399999998</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>404</v>
       </c>
@@ -9511,7 +9521,7 @@
         <v>0.35312995600000002</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>406</v>
       </c>
@@ -9549,7 +9559,7 @@
         <v>0.30976582000000003</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>408</v>
       </c>
@@ -9587,7 +9597,7 @@
         <v>0.193144598</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>410</v>
       </c>
@@ -9625,7 +9635,7 @@
         <v>0.19539134799999999</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>412</v>
       </c>
@@ -9663,7 +9673,7 @@
         <v>0.33073484199999997</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>414</v>
       </c>
@@ -9701,7 +9711,7 @@
         <v>0.33436614799999997</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>416</v>
       </c>
@@ -9739,7 +9749,7 @@
         <v>0.53296923200000001</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>418</v>
       </c>
@@ -9777,7 +9787,7 @@
         <v>0.71832722800000004</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>420</v>
       </c>
@@ -9815,7 +9825,7 @@
         <v>0.19453941299999999</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>422</v>
       </c>
@@ -9853,7 +9863,7 @@
         <v>0.20658236499999999</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>424</v>
       </c>
@@ -9891,7 +9901,7 @@
         <v>0.64060452700000003</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>426</v>
       </c>
@@ -9929,7 +9939,7 @@
         <v>0.25257163300000002</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>428</v>
       </c>
@@ -9967,7 +9977,7 @@
         <v>0.21258152499999999</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>430</v>
       </c>
@@ -10005,7 +10015,7 @@
         <v>0.84421047400000004</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>432</v>
       </c>
@@ -10043,7 +10053,7 @@
         <v>0.19454253799999999</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>434</v>
       </c>
@@ -10081,7 +10091,7 @@
         <v>0.210923315</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>436</v>
       </c>
@@ -10119,7 +10129,7 @@
         <v>0.56343069499999998</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>438</v>
       </c>
@@ -10157,7 +10167,7 @@
         <v>0.245712228</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>440</v>
       </c>
@@ -10195,7 +10205,7 @@
         <v>0.26837336499999997</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>442</v>
       </c>
@@ -10233,7 +10243,7 @@
         <v>0.44232325700000003</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>444</v>
       </c>
@@ -10271,7 +10281,7 @@
         <v>0.268439704</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>446</v>
       </c>
@@ -10309,7 +10319,7 @@
         <v>0.25802857200000001</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>448</v>
       </c>
@@ -10347,7 +10357,7 @@
         <v>0.71866595300000002</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>450</v>
       </c>
@@ -10385,7 +10395,7 @@
         <v>0.20298744899999999</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>452</v>
       </c>
@@ -10423,7 +10433,7 @@
         <v>0.22074221199999999</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>454</v>
       </c>
@@ -10461,7 +10471,7 @@
         <v>0.21834590700000001</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>456</v>
       </c>
@@ -10499,7 +10509,7 @@
         <v>0.49590343999999997</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>458</v>
       </c>
@@ -10537,7 +10547,7 @@
         <v>0.230040625</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>460</v>
       </c>
@@ -10575,7 +10585,7 @@
         <v>0.22603379000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>462</v>
       </c>
@@ -10613,7 +10623,7 @@
         <v>0.99500640900000004</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>464</v>
       </c>
@@ -10651,7 +10661,7 @@
         <v>0.19863646900000001</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>466</v>
       </c>
@@ -10689,7 +10699,7 @@
         <v>0.25795229400000003</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>468</v>
       </c>
@@ -10727,7 +10737,7 @@
         <v>0.234779407</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>470</v>
       </c>
@@ -10765,7 +10775,7 @@
         <v>0.22868772100000001</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>472</v>
       </c>
@@ -10803,7 +10813,7 @@
         <v>0.20074213199999999</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>474</v>
       </c>
@@ -10841,7 +10851,7 @@
         <v>0.201315412</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>476</v>
       </c>
@@ -10879,7 +10889,7 @@
         <v>0.40873564800000001</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>478</v>
       </c>
@@ -10917,7 +10927,7 @@
         <v>0.33625572199999998</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>480</v>
       </c>
@@ -10955,7 +10965,7 @@
         <v>0.38620364499999998</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>482</v>
       </c>
@@ -10993,7 +11003,7 @@
         <v>0.30567097599999998</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>484</v>
       </c>
@@ -11031,7 +11041,7 @@
         <v>0.32492758399999999</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>487</v>
       </c>
@@ -11069,7 +11079,7 @@
         <v>0.86173392699999996</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>489</v>
       </c>
@@ -11107,7 +11117,7 @@
         <v>0.25715539599999998</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>491</v>
       </c>
@@ -11145,7 +11155,7 @@
         <v>0.27437367800000001</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>493</v>
       </c>
@@ -11183,7 +11193,7 @@
         <v>0.19658705700000001</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>495</v>
       </c>
@@ -11221,7 +11231,7 @@
         <v>0.24739223499999999</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>497</v>
       </c>
@@ -11259,7 +11269,7 @@
         <v>0.28286190300000003</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>499</v>
       </c>
@@ -11297,7 +11307,7 @@
         <v>0.193452291</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>501</v>
       </c>
@@ -11335,7 +11345,7 @@
         <v>0.23563063300000001</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>503</v>
       </c>
@@ -11373,7 +11383,7 @@
         <v>0.32773430799999997</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>505</v>
       </c>
@@ -11411,7 +11421,7 @@
         <v>0.28752050800000001</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>507</v>
       </c>
@@ -11449,7 +11459,7 @@
         <v>0.18905708600000001</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>509</v>
       </c>
@@ -11487,7 +11497,7 @@
         <v>0.303377275</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>511</v>
       </c>
@@ -11525,7 +11535,7 @@
         <v>0.80586839099999996</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>513</v>
       </c>
@@ -11563,7 +11573,7 @@
         <v>0.24078201599999999</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>515</v>
       </c>
@@ -11601,7 +11611,7 @@
         <v>0.23030685000000001</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>517</v>
       </c>
@@ -11639,7 +11649,7 @@
         <v>0.19079539100000001</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>519</v>
       </c>
@@ -11677,7 +11687,7 @@
         <v>0.47738814800000001</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>521</v>
       </c>
@@ -11715,7 +11725,7 @@
         <v>0.20032677700000001</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>523</v>
       </c>
@@ -11753,7 +11763,7 @@
         <v>0.28417725999999999</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>525</v>
       </c>
@@ -11791,7 +11801,7 @@
         <v>0.198620242</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>527</v>
       </c>
@@ -11829,7 +11839,7 @@
         <v>0.21619390699999999</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>529</v>
       </c>
@@ -11867,7 +11877,7 @@
         <v>0.192800104</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>531</v>
       </c>
@@ -11905,7 +11915,7 @@
         <v>0.42345578499999997</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>533</v>
       </c>
@@ -11943,7 +11953,7 @@
         <v>0.25925051500000001</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>535</v>
       </c>
@@ -11982,6 +11992,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>